<commit_message>
Update experiments and add optm dsm.
</commit_message>
<xml_diff>
--- a/results/execution/knn_optm_res/knn_optm_res.xlsx
+++ b/results/execution/knn_optm_res/knn_optm_res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marim\CLionProjects\knn_ensemble_research\results\execution\knn_optm_res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BFA4AC-CC75-4E57-AF0E-13978B2F457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDCF5A5-AB6C-4D50-8412-02EA010248A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2848,7 +2848,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,7 +2933,7 @@
         <v>79.4619</v>
       </c>
       <c r="K2" s="3">
-        <v>82.352900000000005</v>
+        <v>82.314300000000003</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>111</v>
@@ -2971,7 +2971,7 @@
         <v>88.492099999999994</v>
       </c>
       <c r="K3" s="3">
-        <v>92.6</v>
+        <v>92.277799999999999</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>112</v>
@@ -3009,7 +3009,7 @@
         <v>92.324100000000001</v>
       </c>
       <c r="K4" s="3">
-        <v>92.1143</v>
+        <v>92.074100000000001</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>113</v>
@@ -3085,7 +3085,7 @@
         <v>84.381299999999996</v>
       </c>
       <c r="K6" s="3">
-        <v>85.763199999999998</v>
+        <v>85.677899999999994</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>115</v>
@@ -3123,7 +3123,7 @@
         <v>80.551699999999997</v>
       </c>
       <c r="K7" s="3">
-        <v>83.488100000000003</v>
+        <v>83.454099999999997</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>116</v>
@@ -3161,7 +3161,7 @@
         <v>96.479500000000002</v>
       </c>
       <c r="K8" s="3">
-        <v>95.0702</v>
+        <v>98.414199999999994</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>117</v>
@@ -3323,7 +3323,7 @@
         <v>75.628600000000006</v>
       </c>
       <c r="K14" s="3">
-        <v>78.176500000000004</v>
+        <v>78.009500000000003</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>120</v>
@@ -3361,7 +3361,7 @@
         <v>87.460300000000004</v>
       </c>
       <c r="K15" s="3">
-        <v>88.15</v>
+        <v>87.896799999999999</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>121</v>
@@ -3399,7 +3399,7 @@
         <v>85.106399999999994</v>
       </c>
       <c r="K16" s="6">
-        <v>91.8</v>
+        <v>91.796300000000002</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>122</v>
@@ -3475,7 +3475,7 @@
         <v>80.213700000000003</v>
       </c>
       <c r="K18" s="3">
-        <v>84.486800000000002</v>
+        <v>84.372600000000006</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>124</v>
@@ -3513,7 +3513,7 @@
         <v>79.104299999999995</v>
       </c>
       <c r="K19" s="3">
-        <v>80.107100000000003</v>
+        <v>80.050399999999996</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>125</v>
@@ -3551,7 +3551,7 @@
         <v>95.949299999999994</v>
       </c>
       <c r="K20" s="3">
-        <v>97.303600000000003</v>
+        <v>97.208600000000004</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>126</v>
@@ -3715,7 +3715,7 @@
         <v>77.685699999999997</v>
       </c>
       <c r="K26" s="3">
-        <v>78.2059</v>
+        <v>77.990499999999997</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>129</v>
@@ -3753,7 +3753,7 @@
         <v>83.182500000000005</v>
       </c>
       <c r="K27" s="3">
-        <v>84.5</v>
+        <v>84.087299999999999</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>130</v>
@@ -3791,7 +3791,7 @@
         <v>85.106399999999994</v>
       </c>
       <c r="K28" s="3">
-        <v>90.1143</v>
+        <v>90.092600000000004</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>131</v>
@@ -3867,7 +3867,7 @@
         <v>80.603300000000004</v>
       </c>
       <c r="K30" s="3">
-        <v>82.8947</v>
+        <v>82.941999999999993</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>133</v>
@@ -3905,7 +3905,7 @@
         <v>77.435699999999997</v>
       </c>
       <c r="K31" s="3">
-        <v>79.25</v>
+        <v>79.222899999999996</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>134</v>
@@ -3943,7 +3943,7 @@
         <v>96.305099999999996</v>
       </c>
       <c r="K32" s="3">
-        <v>96.571399999999997</v>
+        <v>96.501000000000005</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Update experiments and optm dsm results.
</commit_message>
<xml_diff>
--- a/results/execution/knn_optm_res/knn_optm_res.xlsx
+++ b/results/execution/knn_optm_res/knn_optm_res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marim\CLionProjects\knn_ensemble_research\results\execution\knn_optm_res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDCF5A5-AB6C-4D50-8412-02EA010248A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B289F12-58C6-4ED5-B54F-A77ADB89896E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,7 +943,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -964,6 +964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2845,10 +2846,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3ABEA48-9D1E-4C16-981C-1D499460DCED}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3199,7 +3200,7 @@
         <v>89.760900000000007</v>
       </c>
       <c r="K9" s="3">
-        <v>90</v>
+        <v>88.909000000000006</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>118</v>
@@ -3589,7 +3590,7 @@
         <v>88.057599999999994</v>
       </c>
       <c r="K21" s="3">
-        <v>88.019000000000005</v>
+        <v>86.635999999999996</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>127</v>
@@ -3981,7 +3982,7 @@
         <v>86.729900000000001</v>
       </c>
       <c r="K33" s="3">
-        <v>87.361900000000006</v>
+        <v>86.446899999999999</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>136</v>
@@ -4027,6 +4028,9 @@
       <c r="M34" s="3" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K40" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>